<commit_message>
Updated MAX31865 calib and updated editor with wifi dropdwn
</commit_message>
<xml_diff>
--- a/src/libSensors/calibrations/MAX31865/calib_MAX31965.xlsx
+++ b/src/libSensors/calibrations/MAX31865/calib_MAX31965.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feranick/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6BEF481C-F6C1-D84A-BB9E-B34F54849F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2398A9-476F-5F47-98D9-ED461015F3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23220" yWindow="7480" windowWidth="28040" windowHeight="17180" xr2:uid="{833567C5-0EB0-F241-A59C-87E9D7224E38}"/>
+    <workbookView xWindow="12620" yWindow="680" windowWidth="28640" windowHeight="18960" xr2:uid="{833567C5-0EB0-F241-A59C-87E9D7224E38}"/>
   </bookViews>
   <sheets>
     <sheet name="calib" sheetId="2" r:id="rId1"/>
@@ -714,10 +714,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>calib!$B$2:$B$23</c:f>
+              <c:f>calib!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -783,16 +783,25 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>42.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>calib!$A$2:$A$23</c:f>
+              <c:f>calib!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -858,6 +867,15 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,7 +1988,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43227B4-9990-E941-8856-D48E392903B0}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -2034,8 +2052,8 @@
         <v>21.4</v>
       </c>
       <c r="D6">
-        <f>SLOPE(B2:B23,A2:A23)</f>
-        <v>1.0010093868451651</v>
+        <f>SLOPE(B2:B29,A2:A29)</f>
+        <v>1.0003650551139662</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2046,8 +2064,8 @@
         <v>21.2</v>
       </c>
       <c r="D7">
-        <f>INTERCEPT(B2:B23,A2:A23)</f>
-        <v>-2.4328986742707279</v>
+        <f>INTERCEPT(B2:B29,A2:A29)</f>
+        <v>-2.3262560180148917</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2176,6 +2194,54 @@
       </c>
       <c r="B23">
         <v>42.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20.7</v>
+      </c>
+      <c r="B24">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21.3</v>
+      </c>
+      <c r="B25">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>21.8</v>
+      </c>
+      <c r="B26">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="B27">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>20.9</v>
+      </c>
+      <c r="B28">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>20.2</v>
+      </c>
+      <c r="B29">
+        <v>17.899999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>